<commit_message>
add invoice column in download file
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Spare Requested Parts.xlsx
+++ b/application/controllers/excel-templates/Spare Requested Parts.xlsx
@@ -11,11 +11,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Customer Name</t>
   </si>
   <si>
+    <t>Invoice Id</t>
+  </si>
+  <si>
     <t>Booking Id</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t>{spare:name}</t>
+  </si>
+  <si>
+    <t>{spare:purchase_invoice_id}</t>
   </si>
   <si>
     <t>{spare:booking_id}</t>
@@ -100,7 +106,9 @@
       <color rgb="FF4B5056"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
-    <font/>
+    <font>
+      <name val="Cambria"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -127,10 +135,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -146,21 +154,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="5" max="5" width="22.0"/>
-    <col customWidth="1" min="6" max="6" width="18.0"/>
-    <col customWidth="1" min="7" max="7" width="26.43"/>
-    <col customWidth="1" min="8" max="8" width="32.57"/>
-    <col customWidth="1" min="9" max="9" width="30.29"/>
-    <col customWidth="1" min="10" max="10" width="22.86"/>
-    <col customWidth="1" min="11" max="11" width="21.43"/>
-    <col customWidth="1" min="12" max="12" width="29.29"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -199,43 +199,49 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>